<commit_message>
Completado Movil - avanzando Hogar
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
+++ b/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>TC1</t>
   </si>
@@ -128,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,46 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -223,7 +263,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -260,7 +300,15 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
@@ -542,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:AK71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="V1" sqref="V1:V2"/>
@@ -703,6 +751,9 @@
       <c r="X2" t="s">
         <v>31</v>
       </c>
+      <c r="AJ2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row customFormat="1" r="3" s="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H3" s="8"/>

</xml_diff>

<commit_message>
HOGAR TRIO - DUO COMPLETADO
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
+++ b/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>TC1</t>
   </si>
@@ -102,9 +102,6 @@
     <t>ARCHIVO_ADJUNTO</t>
   </si>
   <si>
-    <t>C:\Users\alberto.junco\Downloads\screencapture-itsm-tdp-onbmc-arsys-forms-onbmc-s-SHR-LandingConsole-Default-Administrator-View-2020-02-25-20_44_28</t>
-  </si>
-  <si>
     <t>ADJUNTA_RECIBO</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Fui a la sede me Telefonica en San Isidro, en buen estado lo devolvi</t>
+  </si>
+  <si>
+    <t>C:\Users\Naimar.Garcia\Downloads\DocPrueba</t>
   </si>
 </sst>
 </file>
@@ -128,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,81 +150,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -263,7 +188,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -293,22 +218,7 @@
     </xf>
     <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
@@ -592,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="V1" sqref="V1:V2"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,11 +522,12 @@
     <col min="15" max="15" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
     <col min="16" max="16" customWidth="true" width="25.85546875" collapsed="true"/>
     <col min="17" max="17" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" width="146.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="43.140625" collapsed="true"/>
     <col min="21" max="21" customWidth="true" width="61.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,19 +583,19 @@
         <v>26</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -734,67 +645,67 @@
         <v>24</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="T2" s="7">
         <v>100</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AJ2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row customFormat="1" r="3" s="1" spans="1:22" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H3" s="8"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H4" s="8"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H5" s="8"/>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H6" s="8"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H8" s="8"/>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H9" s="8"/>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H10" s="8"/>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H11" s="8"/>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H12" s="8"/>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H13" s="8"/>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H14" s="8"/>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H15" s="8"/>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="H16" s="8"/>
     </row>
     <row customFormat="1" r="17" s="1" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Flujos de reclamos TERMINADO
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
+++ b/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>TC1</t>
   </si>
@@ -128,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,41 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -188,7 +223,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -218,7 +253,14 @@
     </xf>
     <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>

</xml_diff>

<commit_message>
Cambios de consulta de lineas moviles
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
+++ b/web-automation-framework/src/main/resources/excel/Registro Reclamo Hogar Trío.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>TC1</t>
   </si>
@@ -128,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,96 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -223,7 +313,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -260,7 +350,25 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>

</xml_diff>